<commit_message>
validateUsername,validateEmail,testcases added,created test folder, backend
</commit_message>
<xml_diff>
--- a/Testing_Doc/TestCase.xlsx
+++ b/Testing_Doc/TestCase.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtran/Desktop/Advanced-Web-Application-Project/Product/Ad_web_app_project-master/TestCSV/Testing_Doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtran/Desktop/Advanced-Web-Application-Project/Testing_Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F55DC3-F086-9448-BA4E-59FC00309B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2403553-7F6A-3640-AF7D-0808DCCFD58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="76800" windowHeight="43200" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="1620" windowWidth="36060" windowHeight="37640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CoverSheet" sheetId="3" r:id="rId1"/>
-    <sheet name="TestCase01" sheetId="1" r:id="rId2"/>
-    <sheet name="TestCase02" sheetId="5" r:id="rId3"/>
+    <sheet name="TestCase01" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCase02" sheetId="5" r:id="rId2"/>
+    <sheet name="TestCase03" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,90 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
-  <si>
-    <t>Test Case ID:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Test Priority (Low/Medium/High):</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Module Name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <t>Test Title:</t>
-  </si>
-  <si>
-    <t>Description:</t>
-  </si>
-  <si>
-    <t>Test Designed by:</t>
-  </si>
-  <si>
-    <t>Test Designed date:</t>
-  </si>
-  <si>
-    <t>Test Executed by:</t>
-  </si>
-  <si>
-    <t>Test Execution date:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pre-conditions:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Dependencies:</t>
-    </r>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -144,33 +65,7 @@
     <t>Post-conditions:</t>
   </si>
   <si>
-    <t>Test Case ID: 1</t>
-  </si>
-  <si>
     <t>Test Title: Password validation</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Module Name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: server </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Description: Password should contain at least 8 characters  and numbers </t>
@@ -234,6 +129,153 @@
   </si>
   <si>
     <t>passed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Module Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: server , unit testing</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Case ID: 2.2.1</t>
+  </si>
+  <si>
+    <t>Test Case ID: 2.2.2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Module Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Email address validation</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Title: Email Validation</t>
+  </si>
+  <si>
+    <t>Description: The valid email should contain numbers, letters and @ symbol</t>
+  </si>
+  <si>
+    <t>Test Designed date: 19.11.2022</t>
+  </si>
+  <si>
+    <t>Test Execution date: 19.11.2022</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-conditions:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dependencies:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  jest 29.3.1</t>
+    </r>
+  </si>
+  <si>
+    <t>post-condition</t>
+  </si>
+  <si>
+    <t>Test Case ID: 2.2.3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Module Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: User name validation</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Title: Username Validation</t>
+  </si>
+  <si>
+    <t>Description: Check for a valid user name</t>
+  </si>
+  <si>
+    <t>Post-conditions: passed</t>
   </si>
 </sst>
 </file>
@@ -479,6 +521,104 @@
         <a:xfrm>
           <a:off x="304800" y="3721100"/>
           <a:ext cx="7772400" cy="5960001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2057400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>81547</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50A25FD4-3D38-F31A-8C67-95C68DBE5385}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="317500" y="3784600"/>
+          <a:ext cx="7772400" cy="4488447"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>62894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9B58ED5-C3D4-DE64-B231-BA812F4E406C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="279400" y="3670300"/>
+          <a:ext cx="7772400" cy="2488594"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -752,25 +892,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4F4702-8752-433F-9B63-676ADD83FB29}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -796,7 +922,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -806,7 +932,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -816,7 +942,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -826,7 +952,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -836,7 +962,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -846,7 +972,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -856,7 +982,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -874,7 +1000,7 @@
     </row>
     <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -892,25 +1018,25 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
@@ -1025,7 +1151,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1043,10 +1169,10 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1069,11 +1195,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8B1E0C-5059-4085-93FB-99FD6E7A65F9}">
-  <dimension ref="B3:H35"/>
+  <dimension ref="B3:H47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1088,7 +1216,7 @@
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1098,7 +1226,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1108,7 +1236,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="17" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -1118,7 +1246,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1128,7 +1256,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1138,7 +1266,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1148,7 +1276,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1158,7 +1286,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1168,7 +1296,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1178,7 +1306,7 @@
     </row>
     <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -1196,25 +1324,25 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
@@ -1329,7 +1457,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1344,6 +1472,14 @@
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1361,5 +1497,304 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBA9DE6-CB7E-F543-990F-A56658154CE9}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:G35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test case 7 added
</commit_message>
<xml_diff>
--- a/Testing_Doc/TestCase.xlsx
+++ b/Testing_Doc/TestCase.xlsx
@@ -5,17 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtran/Desktop/Advanced-Web-Application-Project/Testing_Doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtran/Desktop/testing_case/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2403553-7F6A-3640-AF7D-0808DCCFD58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56714F6A-44A6-F448-8AB9-134265B366CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1620" windowWidth="36060" windowHeight="37640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31140" yWindow="500" windowWidth="36060" windowHeight="40760" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase01" sheetId="1" r:id="rId1"/>
     <sheet name="TestCase02" sheetId="5" r:id="rId2"/>
     <sheet name="TestCase03" sheetId="6" r:id="rId3"/>
+    <sheet name="TestCase04" sheetId="8" r:id="rId4"/>
+    <sheet name="TestCase05" sheetId="9" r:id="rId5"/>
+    <sheet name="TestCase06" sheetId="10" r:id="rId6"/>
+    <sheet name="TestCase07" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
   <si>
     <t>Test Priority (Low/Medium/High):</t>
   </si>
@@ -276,6 +280,326 @@
   </si>
   <si>
     <t>Post-conditions: passed</t>
+  </si>
+  <si>
+    <t>Test Case ID: 2.3.1</t>
+  </si>
+  <si>
+    <t>Description: Check that created password is hashed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Title: hashed password </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Module Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: password </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-conditions:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dependencies:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <t>create a user's account</t>
+  </si>
+  <si>
+    <t>check database</t>
+  </si>
+  <si>
+    <t>screenshot added</t>
+  </si>
+  <si>
+    <t>register new user</t>
+  </si>
+  <si>
+    <t>jsonwebtoken created</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Test Case ID: 2.3.2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Module Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: jsonwebtoken</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Title: jwt validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description:  jsonwebtoken created </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-conditions:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dependencies:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> postman</t>
+    </r>
+  </si>
+  <si>
+    <t>login with username and pwd</t>
+  </si>
+  <si>
+    <t>Test Title: delete user</t>
+  </si>
+  <si>
+    <t>Test Case ID: 2.3.3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Module Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+  </si>
+  <si>
+    <t>Description: user can delete own account with jsonwebtoken</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>delete account</t>
+  </si>
+  <si>
+    <t>screen shot added</t>
+  </si>
+  <si>
+    <t>user has been deleted</t>
+  </si>
+  <si>
+    <t>Test Case ID: 2.1.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Module Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: UI/UX</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Title: responsiveness</t>
+  </si>
+  <si>
+    <t>Description: UI should scale if the window is resized, and smallest supported window is 600px horizontal.</t>
+  </si>
+  <si>
+    <t>Test Designed date: 25.11.2022</t>
+  </si>
+  <si>
+    <t>register field</t>
+  </si>
+  <si>
+    <t>600px</t>
+  </si>
+  <si>
+    <t>text readable</t>
+  </si>
+  <si>
+    <t>login field</t>
+  </si>
+  <si>
+    <t>600px view</t>
+  </si>
+  <si>
+    <t>main page</t>
+  </si>
+  <si>
+    <t>visualizations readable</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-conditions:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dependencies:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Viewport resizer</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -630,6 +954,378 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12699</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>443812</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F70FF76-AE55-F0BB-8938-DAABE036CF28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12699" y="7188200"/>
+          <a:ext cx="13359713" cy="7797800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>184357</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>187886</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5346BAA7-016C-13E2-5996-F0F04F18AA83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="184357" y="15303500"/>
+          <a:ext cx="12883943" cy="11935386"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3111500</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>163384</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B583615-7A3C-5523-315C-42FE13414D71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="165100" y="12458699"/>
+          <a:ext cx="8978900" cy="6564185"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3076892</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A99ED23-B59D-1C1A-39D1-EC94E5097E42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="292100" y="7099300"/>
+          <a:ext cx="8817292" cy="5207000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>36728</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{559F6170-58AB-8FE1-2D57-00FE978F9BEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="304800" y="7010399"/>
+          <a:ext cx="10668000" cy="5789829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>187401</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2997200</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>116443</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{087DE8E2-37E5-F7E9-ADE5-A7F1094D18DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="187401" y="7150100"/>
+          <a:ext cx="8842299" cy="8396843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3022600</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>118848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{502291B8-9E21-033D-901B-403C7588A7F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="15989299"/>
+          <a:ext cx="8788400" cy="8132549"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>124721</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3053320</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BE5A087-809C-51AE-79FC-E44248DA91FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="292100" y="24508721"/>
+          <a:ext cx="8793720" cy="7177779"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1505,7 +2201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBA9DE6-CB7E-F543-990F-A56658154CE9}">
   <dimension ref="B3:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B34" sqref="B34:G35"/>
     </sheetView>
   </sheetViews>
@@ -1797,4 +2493,1276 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA685612-EF94-F441-8A26-EC5C55B7C8E8}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O119" sqref="O119"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DBE802-B19E-F94C-A022-8F5C2A5850EE}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2345A1F2-5717-FE49-8148-812E105287BD}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695D3CF2-076C-D648-8380-16C84DDC1F17}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B11:G11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Deleted some old stuff that were not needed, added a new test case and modified the chart 7 to show the v10 stuff (Just for the moment) until Kiet can do it
</commit_message>
<xml_diff>
--- a/Testing_Doc/TestCase.xlsx
+++ b/Testing_Doc/TestCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtran/Desktop/testing_case/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jere\Desktop\Current Project\React-Node-MongoDB-Graph-Website\Testing_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56714F6A-44A6-F448-8AB9-134265B366CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8311F2-B0FC-418A-A587-8988FBEC38B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31140" yWindow="500" windowWidth="36060" windowHeight="40760" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase01" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="TestCase05" sheetId="9" r:id="rId5"/>
     <sheet name="TestCase06" sheetId="10" r:id="rId6"/>
     <sheet name="TestCase07" sheetId="11" r:id="rId7"/>
+    <sheet name="TestCase08" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="89">
   <si>
     <t>Test Priority (Low/Medium/High):</t>
   </si>
@@ -600,6 +601,125 @@
       </rPr>
       <t xml:space="preserve"> Viewport resizer</t>
     </r>
+  </si>
+  <si>
+    <t>Test Case ID: 2.3.4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Module Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Chart 7</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Title: Database change effect on chart</t>
+  </si>
+  <si>
+    <t>Description: Chart data should change according to the data changed from DB</t>
+  </si>
+  <si>
+    <t>Test Designed by: Jere Muikku</t>
+  </si>
+  <si>
+    <t>Test Designed date: 26.11.2022</t>
+  </si>
+  <si>
+    <t>Test Executed by: Jere Muikku</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-conditions:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dependencies:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Putting new event to Database</t>
+  </si>
+  <si>
+    <t>Event: Random event</t>
+  </si>
+  <si>
+    <t>Will show up on the year placed, or to the new year added</t>
+  </si>
+  <si>
+    <t>The result is the same as expected</t>
+  </si>
+  <si>
+    <t>Picture added</t>
+  </si>
+  <si>
+    <t>Checking the chart</t>
+  </si>
+  <si>
+    <t>Data from the database with the new event</t>
+  </si>
+  <si>
+    <t>The data is able to be created to DB</t>
+  </si>
+  <si>
+    <t>Deleting the data from database</t>
+  </si>
+  <si>
+    <t>The new data that was put in the DB</t>
+  </si>
+  <si>
+    <t>The test data will be gone from db and the chart</t>
   </si>
 </sst>
 </file>
@@ -1326,6 +1446,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1132273</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>104571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53A7F973-9FC8-3D7A-5EB9-42BAB0D48BF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="6667500"/>
+          <a:ext cx="9619048" cy="1628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2265606</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>170857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8508EEF5-9B8E-4FC4-2069-9C74E89C2031}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="8572500"/>
+          <a:ext cx="10752381" cy="4742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1595,18 +1808,18 @@
       <selection activeCell="B17" sqref="B17:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1616,7 +1829,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1626,7 +1839,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>17</v>
       </c>
@@ -1636,7 +1849,7 @@
       <c r="F6" s="18"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1646,7 +1859,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1656,7 +1869,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1666,7 +1879,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1676,7 +1889,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1686,7 +1899,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1694,7 +1907,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>14</v>
       </c>
@@ -1704,7 +1917,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1712,7 +1925,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1735,7 +1948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>1</v>
       </c>
@@ -1746,7 +1959,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>2</v>
       </c>
@@ -1757,7 +1970,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -1768,7 +1981,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>4</v>
       </c>
@@ -1779,7 +1992,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>5</v>
       </c>
@@ -1790,7 +2003,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>6</v>
       </c>
@@ -1801,7 +2014,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>7</v>
       </c>
@@ -1812,7 +2025,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>8</v>
       </c>
@@ -1823,7 +2036,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>9</v>
       </c>
@@ -1834,7 +2047,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>10</v>
       </c>
@@ -1845,7 +2058,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -1855,7 +2068,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -1863,7 +2076,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>15</v>
       </c>
@@ -1899,18 +2112,18 @@
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1920,7 +2133,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1930,7 +2143,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>20</v>
       </c>
@@ -1940,7 +2153,7 @@
       <c r="F6" s="18"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1950,7 +2163,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1960,7 +2173,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1970,7 +2183,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1980,7 +2193,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1990,7 +2203,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2000,7 +2213,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>25</v>
       </c>
@@ -2010,7 +2223,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -2018,7 +2231,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2041,7 +2254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>1</v>
       </c>
@@ -2052,7 +2265,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>2</v>
       </c>
@@ -2063,7 +2276,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -2074,7 +2287,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>4</v>
       </c>
@@ -2085,7 +2298,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>5</v>
       </c>
@@ -2096,7 +2309,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>6</v>
       </c>
@@ -2107,7 +2320,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>7</v>
       </c>
@@ -2118,7 +2331,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>8</v>
       </c>
@@ -2129,7 +2342,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>9</v>
       </c>
@@ -2140,7 +2353,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>10</v>
       </c>
@@ -2151,7 +2364,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -2161,7 +2374,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -2169,13 +2382,311 @@
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>26</v>
       </c>
       <c r="D47" t="s">
         <v>16</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBA9DE6-CB7E-F543-990F-A56658154CE9}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:G35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2197,28 +2708,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBA9DE6-CB7E-F543-990F-A56658154CE9}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA685612-EF94-F441-8A26-EC5C55B7C8E8}">
   <dimension ref="B3:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:G35"/>
+      <selection activeCell="O119" sqref="O119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2226,7 +2737,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2236,9 +2747,9 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -2246,9 +2757,9 @@
       <c r="F6" s="18"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2256,9 +2767,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2266,7 +2777,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2276,7 +2787,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
@@ -2286,7 +2797,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2296,7 +2807,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2306,9 +2817,9 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -2316,7 +2827,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -2324,7 +2835,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2347,29 +2858,41 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -2380,7 +2903,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>4</v>
       </c>
@@ -2391,7 +2914,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>5</v>
       </c>
@@ -2402,7 +2925,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>6</v>
       </c>
@@ -2413,7 +2936,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>7</v>
       </c>
@@ -2424,7 +2947,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>8</v>
       </c>
@@ -2435,7 +2958,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>9</v>
       </c>
@@ -2446,7 +2969,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>10</v>
       </c>
@@ -2457,7 +2980,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>31</v>
       </c>
@@ -2467,7 +2990,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -2495,28 +3018,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA685612-EF94-F441-8A26-EC5C55B7C8E8}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DBE802-B19E-F94C-A022-8F5C2A5850EE}">
   <dimension ref="B3:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O119" sqref="O119"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2524,7 +3047,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2534,9 +3057,9 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -2544,9 +3067,9 @@
       <c r="F6" s="18"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2554,9 +3077,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2564,7 +3087,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2574,9 +3097,9 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2584,7 +3107,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2594,19 +3117,17 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -2614,7 +3135,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -2622,7 +3143,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2645,41 +3166,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="G22" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="G23" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -2690,7 +3219,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>4</v>
       </c>
@@ -2701,7 +3230,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>5</v>
       </c>
@@ -2712,7 +3241,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>6</v>
       </c>
@@ -2723,7 +3252,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>7</v>
       </c>
@@ -2734,7 +3263,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>8</v>
       </c>
@@ -2745,7 +3274,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>9</v>
       </c>
@@ -2756,7 +3285,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>10</v>
       </c>
@@ -2767,7 +3296,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>31</v>
       </c>
@@ -2777,7 +3306,653 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2345A1F2-5717-FE49-8148-812E105287BD}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695D3CF2-076C-D648-8380-16C84DDC1F17}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -2805,28 +3980,36 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DBE802-B19E-F94C-A022-8F5C2A5850EE}">
-  <dimension ref="B3:H35"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED1F754-0260-477A-8FAC-3B8DAA168FEF}">
+  <dimension ref="B2:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="64" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2834,29 +4017,29 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2864,19 +4047,19 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -2884,120 +4067,135 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
       <c r="C21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
         <v>2</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="E22" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="E23" s="1" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -3006,9 +4204,9 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -3017,9 +4215,9 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -3028,9 +4226,9 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -3039,9 +4237,9 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -3050,9 +4248,9 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -3061,9 +4259,9 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -3072,697 +4270,39 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="1">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G17"/>
+    <mergeCell ref="B33:G34"/>
+    <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2345A1F2-5717-FE49-8148-812E105287BD}">
-  <dimension ref="B3:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="64" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="1">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="1">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="1">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="1">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="1">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="1">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="1">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B34:G35"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695D3CF2-076C-D648-8380-16C84DDC1F17}">
-  <dimension ref="B3:H35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="64" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="1">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="1">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="1">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="1">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="1">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="1">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="1">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B34:G35"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B11:G11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished test case, should be the last commit, probably
</commit_message>
<xml_diff>
--- a/Testing_Doc/TestCase.xlsx
+++ b/Testing_Doc/TestCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtran/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jere\Advanced Web Application Project\Testing_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70695635-00FE-C644-8B6B-5666FF2B7760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C045B41-F1BF-4ABA-BECF-F3970ABA9252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38640" windowHeight="21840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase01" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="118">
   <si>
     <t>Test Priority (Low/Medium/High):</t>
   </si>
@@ -747,12 +747,6 @@
     </r>
   </si>
   <si>
-    <t>Test Title: Chart data to database and Frontend (when done)</t>
-  </si>
-  <si>
-    <t>UPDATE LATER WHEN THE FRONTEND SIDE IS DONE</t>
-  </si>
-  <si>
     <t>Test Designed date: 29.11.2022</t>
   </si>
   <si>
@@ -837,6 +831,24 @@
   </si>
   <si>
     <t>login with registed account</t>
+  </si>
+  <si>
+    <t>Step 4 again</t>
+  </si>
+  <si>
+    <t>Result is as expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Title: Chart data to database and Frontend </t>
+  </si>
+  <si>
+    <t>Chart shows up on the frontend</t>
+  </si>
+  <si>
+    <t>New chart array data</t>
+  </si>
+  <si>
+    <t>Chart shows on the frontend with the new id when searched</t>
   </si>
 </sst>
 </file>
@@ -2015,6 +2027,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2779315</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>112724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02C306EC-EAE1-0391-F266-E4746E7006DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="295275" y="26555700"/>
+          <a:ext cx="15876190" cy="12609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2287,18 +2343,18 @@
       <selection activeCell="B17" sqref="B17:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -2308,7 +2364,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2318,7 +2374,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>17</v>
       </c>
@@ -2328,7 +2384,7 @@
       <c r="F6" s="18"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -2338,7 +2394,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2348,7 +2404,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2358,7 +2414,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -2368,7 +2424,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2378,7 +2434,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2386,7 +2442,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>14</v>
       </c>
@@ -2396,7 +2452,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -2404,7 +2460,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2427,7 +2483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>1</v>
       </c>
@@ -2438,7 +2494,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>2</v>
       </c>
@@ -2449,7 +2505,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -2460,7 +2516,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>4</v>
       </c>
@@ -2471,7 +2527,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>5</v>
       </c>
@@ -2482,7 +2538,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>6</v>
       </c>
@@ -2493,7 +2549,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>7</v>
       </c>
@@ -2504,7 +2560,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>8</v>
       </c>
@@ -2515,7 +2571,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>9</v>
       </c>
@@ -2526,7 +2582,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>10</v>
       </c>
@@ -2537,7 +2593,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -2547,7 +2603,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -2555,7 +2611,7 @@
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>15</v>
       </c>
@@ -2587,24 +2643,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421545EC-9779-C644-8BD7-FFF9102B26CE}">
   <dimension ref="B3:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2612,7 +2668,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2622,9 +2678,9 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -2632,9 +2688,9 @@
       <c r="F6" s="18"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2642,9 +2698,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2652,7 +2708,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2662,7 +2718,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -2672,7 +2728,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2682,7 +2738,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2690,7 +2746,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>77</v>
       </c>
@@ -2700,7 +2756,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -2708,7 +2764,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2731,40 +2787,40 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>42</v>
@@ -2773,7 +2829,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -2784,7 +2840,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>4</v>
       </c>
@@ -2795,7 +2851,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>5</v>
       </c>
@@ -2806,7 +2862,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>6</v>
       </c>
@@ -2817,7 +2873,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>7</v>
       </c>
@@ -2828,7 +2884,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>8</v>
       </c>
@@ -2839,7 +2895,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>9</v>
       </c>
@@ -2850,7 +2906,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>10</v>
       </c>
@@ -2861,7 +2917,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -2871,7 +2927,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -2879,13 +2935,617 @@
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>15</v>
       </c>
       <c r="D54" t="s">
         <v>16</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8B1E0C-5059-4085-93FB-99FD6E7A65F9}">
+  <dimension ref="B3:H47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBA9DE6-CB7E-F543-990F-A56658154CE9}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:G35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2907,28 +3567,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8B1E0C-5059-4085-93FB-99FD6E7A65F9}">
-  <dimension ref="B3:H47"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA685612-EF94-F441-8A26-EC5C55B7C8E8}">
+  <dimension ref="B3:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="O119" sqref="O119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2936,7 +3596,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2946,9 +3606,9 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -2956,9 +3616,9 @@
       <c r="F6" s="18"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2966,9 +3626,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2976,7 +3636,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2986,7 +3646,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
@@ -2996,7 +3656,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -3006,7 +3666,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -3016,9 +3676,9 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -3026,7 +3686,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -3034,7 +3694,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -3057,29 +3717,41 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -3090,7 +3762,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>4</v>
       </c>
@@ -3101,7 +3773,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>5</v>
       </c>
@@ -3112,7 +3784,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>6</v>
       </c>
@@ -3123,7 +3795,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>7</v>
       </c>
@@ -3134,7 +3806,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>8</v>
       </c>
@@ -3145,7 +3817,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>9</v>
       </c>
@@ -3156,7 +3828,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>10</v>
       </c>
@@ -3167,9 +3839,9 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -3177,7 +3849,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -3185,13 +3857,967 @@
       <c r="F35" s="9"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" t="s">
-        <v>16</v>
-      </c>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DBE802-B19E-F94C-A022-8F5C2A5850EE}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2345A1F2-5717-FE49-8148-812E105287BD}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695D3CF2-076C-D648-8380-16C84DDC1F17}">
+  <dimension ref="B3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3213,1576 +4839,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBA9DE6-CB7E-F543-990F-A56658154CE9}">
-  <dimension ref="B3:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:G35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="64" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="1">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="1">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="1">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="1">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="1">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="1">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="1">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B34:G35"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA685612-EF94-F441-8A26-EC5C55B7C8E8}">
-  <dimension ref="B3:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O119" sqref="O119"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="64" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="1">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="1">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="1">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="1">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="1">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="1">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="1">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B34:G35"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DBE802-B19E-F94C-A022-8F5C2A5850EE}">
-  <dimension ref="B3:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="64" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="1">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="1">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="1">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="1">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="1">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="1">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="1">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B34:G35"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2345A1F2-5717-FE49-8148-812E105287BD}">
-  <dimension ref="B3:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="64" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="1">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="1">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="1">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="1">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="1">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="1">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="1">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B34:G35"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695D3CF2-076C-D648-8380-16C84DDC1F17}">
-  <dimension ref="B3:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:G18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="64" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="1">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="1">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="1">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="1">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="1">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="1">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="1">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B34:G35"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED1F754-0260-477A-8FAC-3B8DAA168FEF}">
   <dimension ref="B2:H34"/>
@@ -4791,16 +4847,16 @@
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>57</v>
       </c>
@@ -4810,7 +4866,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -4820,7 +4876,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>71</v>
       </c>
@@ -4830,7 +4886,7 @@
       <c r="F5" s="18"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>72</v>
       </c>
@@ -4840,7 +4896,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>73</v>
       </c>
@@ -4850,7 +4906,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>74</v>
       </c>
@@ -4860,7 +4916,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>75</v>
       </c>
@@ -4870,7 +4926,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>76</v>
       </c>
@@ -4880,7 +4936,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -4888,7 +4944,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>77</v>
       </c>
@@ -4898,7 +4954,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -4906,7 +4962,7 @@
       <c r="F17" s="15"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
@@ -4929,7 +4985,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>1</v>
       </c>
@@ -4952,7 +5008,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>2</v>
       </c>
@@ -4975,7 +5031,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -4996,7 +5052,7 @@
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>4</v>
       </c>
@@ -5007,7 +5063,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>5</v>
       </c>
@@ -5018,7 +5074,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>6</v>
       </c>
@@ -5029,7 +5085,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>7</v>
       </c>
@@ -5040,7 +5096,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>8</v>
       </c>
@@ -5051,7 +5107,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>9</v>
       </c>
@@ -5062,7 +5118,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>10</v>
       </c>
@@ -5073,7 +5129,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>8</v>
       </c>
@@ -5083,7 +5139,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -5093,17 +5149,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G17"/>
+    <mergeCell ref="B33:G34"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B16:G17"/>
-    <mergeCell ref="B33:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5114,20 +5170,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0788FFA-244C-432B-AD3F-080798A87D75}">
   <dimension ref="B1:H30"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="58" customWidth="1"/>
-    <col min="5" max="5" width="59.5" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" customWidth="1"/>
-    <col min="7" max="7" width="45.5" customWidth="1"/>
+    <col min="5" max="5" width="59.42578125" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="7" max="7" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="17" t="s">
         <v>89</v>
       </c>
@@ -5137,9 +5193,9 @@
       <c r="F1" s="18"/>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -5147,7 +5203,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>73</v>
       </c>
@@ -5157,12 +5213,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>74</v>
       </c>
@@ -5172,9 +5223,9 @@
       <c r="F6" s="3"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -5182,7 +5233,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>76</v>
       </c>
@@ -5192,7 +5243,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -5200,7 +5251,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>77</v>
       </c>
@@ -5210,7 +5261,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -5218,7 +5269,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -5241,18 +5292,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>81</v>
@@ -5264,18 +5315,18 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>81</v>
@@ -5287,18 +5338,18 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>81</v>
@@ -5307,55 +5358,77 @@
         <v>42</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>5</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>6</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>7</v>
       </c>
@@ -5366,7 +5439,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>8</v>
       </c>
@@ -5377,7 +5450,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>9</v>
       </c>
@@ -5388,7 +5461,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>10</v>
       </c>
@@ -5399,7 +5472,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>8</v>
       </c>
@@ -5409,7 +5482,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>

</xml_diff>